<commit_message>
update with new filtering params
</commit_message>
<xml_diff>
--- a/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
+++ b/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/03.var_calling/variant_stats/filtered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E152F8-A962-426E-8D2B-EE3A5787727C}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A2852D9-F406-4E7C-A6D9-389CF8FAC0D4}"/>
   <bookViews>
     <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,17 +559,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="7">
-        <v>94208</v>
+        <v>104238</v>
       </c>
       <c r="C2" s="7">
-        <v>6629</v>
+        <v>7332</v>
       </c>
       <c r="D2" s="8">
-        <v>683353</v>
+        <v>683245</v>
       </c>
       <c r="E2" s="9">
         <f>SUM(B2:D2)</f>
-        <v>784190</v>
+        <v>794815</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -577,17 +577,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>93874</v>
+        <v>103048</v>
       </c>
       <c r="C3" s="7">
-        <v>6348</v>
+        <v>6937</v>
       </c>
       <c r="D3" s="8">
-        <v>736829</v>
+        <v>736819</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ref="E3:E14" si="0">SUM(B3:D3)</f>
-        <v>837051</v>
+        <v>846804</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -595,17 +595,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>98506</v>
+        <v>109888</v>
       </c>
       <c r="C4" s="7">
-        <v>7507</v>
+        <v>8372</v>
       </c>
       <c r="D4" s="8">
-        <v>626764</v>
+        <v>626633</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>732777</v>
+        <v>744893</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -613,17 +613,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>74748</v>
+        <v>82161</v>
       </c>
       <c r="C5" s="7">
-        <v>5269</v>
+        <v>5778</v>
       </c>
       <c r="D5" s="8">
-        <v>537995</v>
+        <v>537914</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
-        <v>618012</v>
+        <v>625853</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -631,17 +631,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>88333</v>
+        <v>97546</v>
       </c>
       <c r="C6" s="7">
-        <v>6879</v>
+        <v>7571</v>
       </c>
       <c r="D6" s="8">
-        <v>523222</v>
+        <v>523135</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>618434</v>
+        <v>628252</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -649,17 +649,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>112605</v>
+        <v>123996</v>
       </c>
       <c r="C7" s="7">
-        <v>7415</v>
+        <v>8191</v>
       </c>
       <c r="D7" s="8">
-        <v>955597</v>
+        <v>955530</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>1075617</v>
+        <v>1087717</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -667,17 +667,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>83908</v>
+        <v>92488</v>
       </c>
       <c r="C8" s="7">
-        <v>6212</v>
+        <v>6829</v>
       </c>
       <c r="D8" s="8">
-        <v>569128</v>
+        <v>568958</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="0"/>
-        <v>659248</v>
+        <v>668275</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -685,17 +685,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>133239</v>
+        <v>146636</v>
       </c>
       <c r="C9" s="7">
-        <v>9648</v>
+        <v>10611</v>
       </c>
       <c r="D9" s="8">
-        <v>891142</v>
+        <v>891010</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="0"/>
-        <v>1034029</v>
+        <v>1048257</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,17 +703,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="7">
-        <v>83253</v>
+        <v>91529</v>
       </c>
       <c r="C10" s="7">
-        <v>5795</v>
+        <v>6354</v>
       </c>
       <c r="D10" s="8">
-        <v>597364</v>
+        <v>597264</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
-        <v>686412</v>
+        <v>695147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -721,17 +721,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>87633</v>
+        <v>96497</v>
       </c>
       <c r="C11" s="7">
-        <v>5973</v>
+        <v>6577</v>
       </c>
       <c r="D11" s="8">
-        <v>683678</v>
+        <v>683599</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="0"/>
-        <v>777284</v>
+        <v>786673</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -739,17 +739,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="7">
-        <v>84984</v>
+        <v>93300</v>
       </c>
       <c r="C12" s="7">
-        <v>5635</v>
+        <v>6134</v>
       </c>
       <c r="D12" s="8">
-        <v>680985</v>
+        <v>680939</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>771604</v>
+        <v>780373</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -757,17 +757,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="10">
-        <v>1552</v>
+        <v>4191</v>
       </c>
       <c r="C13" s="10">
-        <v>354</v>
+        <v>436</v>
       </c>
       <c r="D13" s="11">
-        <v>18578</v>
+        <v>19054</v>
       </c>
       <c r="E13" s="12">
         <f t="shared" si="0"/>
-        <v>20484</v>
+        <v>23681</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -776,19 +776,19 @@
       </c>
       <c r="B14" s="13">
         <f>SUM(B2:B13)</f>
-        <v>1036843</v>
+        <v>1145518</v>
       </c>
       <c r="C14" s="13">
         <f>SUM(C2:C13)</f>
-        <v>73664</v>
+        <v>81122</v>
       </c>
       <c r="D14" s="14">
         <f>SUM(D2:D13)</f>
-        <v>7504635</v>
+        <v>7504100</v>
       </c>
       <c r="E14" s="15">
         <f t="shared" si="0"/>
-        <v>8615142</v>
+        <v>8730740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove indels from invariants
</commit_message>
<xml_diff>
--- a/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
+++ b/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/03.var_calling/variant_stats/filtered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A2852D9-F406-4E7C-A6D9-389CF8FAC0D4}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F67CD9B5-3C47-45AD-85D0-1B7E70E37867}"/>
   <bookViews>
-    <workbookView xWindow="1308" yWindow="-108" windowWidth="21840" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21795" yWindow="-9870" windowWidth="21600" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtered Stats" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,17 +559,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="7">
-        <v>104238</v>
+        <v>104205</v>
       </c>
       <c r="C2" s="7">
-        <v>7332</v>
+        <v>7321</v>
       </c>
       <c r="D2" s="8">
-        <v>683245</v>
+        <v>683440</v>
       </c>
       <c r="E2" s="9">
         <f>SUM(B2:D2)</f>
-        <v>794815</v>
+        <v>794966</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -577,17 +577,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>103048</v>
+        <v>103032</v>
       </c>
       <c r="C3" s="7">
-        <v>6937</v>
+        <v>6933</v>
       </c>
       <c r="D3" s="8">
-        <v>736819</v>
+        <v>736948</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ref="E3:E14" si="0">SUM(B3:D3)</f>
-        <v>846804</v>
+        <v>846913</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -595,17 +595,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>109888</v>
+        <v>109859</v>
       </c>
       <c r="C4" s="7">
-        <v>8372</v>
+        <v>8366</v>
       </c>
       <c r="D4" s="8">
-        <v>626633</v>
+        <v>626870</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>744893</v>
+        <v>745095</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -613,17 +613,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>82161</v>
+        <v>82132</v>
       </c>
       <c r="C5" s="7">
-        <v>5778</v>
+        <v>5771</v>
       </c>
       <c r="D5" s="8">
-        <v>537914</v>
+        <v>538119</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
-        <v>625853</v>
+        <v>626022</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -631,17 +631,17 @@
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>97546</v>
+        <v>97517</v>
       </c>
       <c r="C6" s="7">
-        <v>7571</v>
+        <v>7564</v>
       </c>
       <c r="D6" s="8">
-        <v>523135</v>
+        <v>523321</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>628252</v>
+        <v>628402</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -649,17 +649,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>123996</v>
+        <v>123970</v>
       </c>
       <c r="C7" s="7">
         <v>8191</v>
       </c>
       <c r="D7" s="8">
-        <v>955530</v>
+        <v>955746</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>1087717</v>
+        <v>1087907</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -667,17 +667,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>92488</v>
+        <v>92452</v>
       </c>
       <c r="C8" s="7">
-        <v>6829</v>
+        <v>6822</v>
       </c>
       <c r="D8" s="8">
-        <v>568958</v>
+        <v>569203</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="0"/>
-        <v>668275</v>
+        <v>668477</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -685,17 +685,17 @@
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>146636</v>
+        <v>146604</v>
       </c>
       <c r="C9" s="7">
-        <v>10611</v>
+        <v>10603</v>
       </c>
       <c r="D9" s="8">
-        <v>891010</v>
+        <v>891241</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="0"/>
-        <v>1048257</v>
+        <v>1048448</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -703,17 +703,17 @@
         <v>8</v>
       </c>
       <c r="B10" s="7">
-        <v>91529</v>
+        <v>91501</v>
       </c>
       <c r="C10" s="7">
-        <v>6354</v>
+        <v>6347</v>
       </c>
       <c r="D10" s="8">
-        <v>597264</v>
+        <v>597460</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
-        <v>695147</v>
+        <v>695308</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -721,17 +721,17 @@
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>96497</v>
+        <v>96478</v>
       </c>
       <c r="C11" s="7">
-        <v>6577</v>
+        <v>6575</v>
       </c>
       <c r="D11" s="8">
-        <v>683599</v>
+        <v>683749</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="0"/>
-        <v>786673</v>
+        <v>786802</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -739,17 +739,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="7">
-        <v>93300</v>
+        <v>93288</v>
       </c>
       <c r="C12" s="7">
-        <v>6134</v>
+        <v>6132</v>
       </c>
       <c r="D12" s="8">
-        <v>680939</v>
+        <v>681067</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>780373</v>
+        <v>780487</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -757,17 +757,17 @@
         <v>11</v>
       </c>
       <c r="B13" s="10">
-        <v>4191</v>
+        <v>4181</v>
       </c>
       <c r="C13" s="10">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D13" s="11">
-        <v>19054</v>
+        <v>19068</v>
       </c>
       <c r="E13" s="12">
         <f t="shared" si="0"/>
-        <v>23681</v>
+        <v>23683</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -776,19 +776,19 @@
       </c>
       <c r="B14" s="13">
         <f>SUM(B2:B13)</f>
-        <v>1145518</v>
+        <v>1145219</v>
       </c>
       <c r="C14" s="13">
         <f>SUM(C2:C13)</f>
-        <v>81122</v>
+        <v>81059</v>
       </c>
       <c r="D14" s="14">
         <f>SUM(D2:D13)</f>
-        <v>7504100</v>
+        <v>7506232</v>
       </c>
       <c r="E14" s="15">
         <f t="shared" si="0"/>
-        <v>8730740</v>
+        <v>8732510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
var calling without outgroup
</commit_message>
<xml_diff>
--- a/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
+++ b/03.var_calling/variant_stats/filtered/filtered_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/kasey_pham_ufl_edu/Documents/Grad School Documents/Projects/eucalyptus-hybrid-resequencing/03.var_calling/variant_stats/filtered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AA279BD-3C0D-4058-B717-61C5EC8E988D}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="11_F25DC773A252ABDACC1048CC295F61E45BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9920CED-652B-4728-A170-6CF10415D99E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1800" yWindow="384" windowWidth="19572" windowHeight="12276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24900" yWindow="-8430" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtered Stats" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>chr01</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Num Invariants</t>
+  </si>
+  <si>
+    <t>Without Multiallelic SNPs</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -242,6 +245,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,9 +541,11 @@
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>13</v>
@@ -554,241 +560,248 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
-        <v>104205</v>
+        <v>165262</v>
       </c>
       <c r="C2" s="7">
-        <v>7321</v>
+        <v>9416</v>
       </c>
       <c r="D2" s="8">
-        <v>683440</v>
+        <v>1259181</v>
       </c>
       <c r="E2" s="9">
         <f>SUM(B2:D2)</f>
-        <v>794966</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1433859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>103032</v>
+        <v>167481</v>
       </c>
       <c r="C3" s="7">
-        <v>6933</v>
+        <v>9231</v>
       </c>
       <c r="D3" s="8">
-        <v>736948</v>
+        <v>1368061</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ref="E3:E14" si="0">SUM(B3:D3)</f>
-        <v>846913</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1544773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="7">
-        <v>109859</v>
+        <v>178061</v>
       </c>
       <c r="C4" s="7">
-        <v>8366</v>
+        <v>11455</v>
       </c>
       <c r="D4" s="8">
-        <v>626870</v>
+        <v>1180563</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>745095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1370079</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="7">
-        <v>82132</v>
+        <v>130871</v>
       </c>
       <c r="C5" s="7">
-        <v>5771</v>
+        <v>7412</v>
       </c>
       <c r="D5" s="8">
-        <v>538119</v>
+        <v>1002216</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
-        <v>626022</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1140499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="7">
-        <v>97517</v>
+        <v>160414</v>
       </c>
       <c r="C6" s="7">
-        <v>7564</v>
+        <v>10443</v>
       </c>
       <c r="D6" s="8">
-        <v>523321</v>
+        <v>981011</v>
       </c>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>628402</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1151868</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="7">
-        <v>123970</v>
+        <v>196142</v>
       </c>
       <c r="C7" s="7">
-        <v>8191</v>
+        <v>10318</v>
       </c>
       <c r="D7" s="8">
-        <v>955746</v>
+        <v>1748766</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>1087907</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1955226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="7">
-        <v>92452</v>
+        <v>150019</v>
       </c>
       <c r="C8" s="7">
-        <v>6822</v>
+        <v>9309</v>
       </c>
       <c r="D8" s="8">
-        <v>569203</v>
+        <v>1058566</v>
       </c>
       <c r="E8" s="9">
         <f t="shared" si="0"/>
-        <v>668477</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1217894</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="7">
-        <v>146604</v>
+        <v>236520</v>
       </c>
       <c r="C9" s="7">
-        <v>10603</v>
+        <v>14122</v>
       </c>
       <c r="D9" s="8">
-        <v>891241</v>
+        <v>1654303</v>
       </c>
       <c r="E9" s="9">
         <f t="shared" si="0"/>
-        <v>1048448</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1904945</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="7">
-        <v>91501</v>
+        <v>144600</v>
       </c>
       <c r="C10" s="7">
-        <v>6347</v>
+        <v>7985</v>
       </c>
       <c r="D10" s="8">
-        <v>597460</v>
+        <v>1104510</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
-        <v>695308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1257095</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7">
-        <v>96478</v>
+        <v>153849</v>
       </c>
       <c r="C11" s="7">
-        <v>6575</v>
+        <v>8426</v>
       </c>
       <c r="D11" s="8">
-        <v>683749</v>
+        <v>1258706</v>
       </c>
       <c r="E11" s="9">
         <f t="shared" si="0"/>
-        <v>786802</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1420981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="7">
-        <v>93288</v>
+        <v>149538</v>
       </c>
       <c r="C12" s="7">
-        <v>6132</v>
+        <v>8141</v>
       </c>
       <c r="D12" s="8">
-        <v>681067</v>
+        <v>1262938</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
-        <v>780487</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1420617</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="10">
-        <v>4181</v>
+        <v>7082</v>
       </c>
       <c r="C13" s="10">
-        <v>434</v>
+        <v>657</v>
       </c>
       <c r="D13" s="11">
-        <v>19068</v>
+        <v>34194</v>
       </c>
       <c r="E13" s="12">
         <f t="shared" si="0"/>
-        <v>23683</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41933</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="13">
         <f>SUM(B2:B13)</f>
-        <v>1145219</v>
+        <v>1839839</v>
       </c>
       <c r="C14" s="13">
         <f>SUM(C2:C13)</f>
-        <v>81059</v>
+        <v>106915</v>
       </c>
       <c r="D14" s="14">
         <f>SUM(D2:D13)</f>
-        <v>7506232</v>
+        <v>13913015</v>
       </c>
       <c r="E14" s="15">
         <f t="shared" si="0"/>
-        <v>8732510</v>
+        <v>15859769</v>
+      </c>
+      <c r="F14" s="15">
+        <f>B14+D14</f>
+        <v>15752854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>